<commit_message>
iniciando criação das tabelas
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable-Mod.xlsx
+++ b/SpotifyClone-Non-NormalizedTable-Mod.xlsx
@@ -5,13 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="tabela_usuario" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="tabela_plano" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="tabela_historico_de _reproduçõe" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="tabela_seguindo_artistas" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="tabela_artista" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="tabela_album" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="tabela_canções" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="114">
   <si>
     <t xml:space="preserve">usuario_id</t>
   </si>
@@ -303,7 +307,7 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">musica</t>
+    <t xml:space="preserve">music_id</t>
   </si>
   <si>
     <t xml:space="preserve">"2022-02-28 10:45:55"</t>
@@ -343,6 +347,30 @@
   </si>
   <si>
     <t xml:space="preserve">"2017-10-12 12:35:20"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1; 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1; 2 ; 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5; 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álbuns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jazz, Hot Space </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falso Brilhante, Vento de Maio </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ALIEN SUPERSTAR"</t>
   </si>
 </sst>
 </file>
@@ -560,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8725,7 +8753,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9272,4 +9300,1299 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.56"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.73"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:X11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>279</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>369</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>116</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>203</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>152</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>105</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>207</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>267</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>244</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>